<commit_message>
add 2014 conodont Sr data, new equation to calculate hydrothermal flux
</commit_message>
<xml_diff>
--- a/Data/OrdoGTS2020.xlsx
+++ b/Data/OrdoGTS2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datua\!Notebook\avila_etal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C31468-777E-448A-B8E1-30A5E12ED228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C707E6-D3B2-4784-AB8B-5978A5251260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11715" xr2:uid="{1B88487C-DC49-4324-B729-938B2EA86772}"/>
+    <workbookView xWindow="3450" yWindow="1830" windowWidth="21600" windowHeight="11715" xr2:uid="{1B88487C-DC49-4324-B729-938B2EA86772}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>445.21</v>

</xml_diff>